<commit_message>
fixed errors in part numbering
</commit_message>
<xml_diff>
--- a/Part nr. full assembled smfScope up to date.xlsx
+++ b/Part nr. full assembled smfScope up to date.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Excitation path" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="209">
   <si>
     <t>Part Nr.</t>
   </si>
@@ -124,15 +124,6 @@
     <t>RS1.5P/M</t>
   </si>
   <si>
-    <t>Post holder collimating lens</t>
-  </si>
-  <si>
-    <t>Post collimating lens</t>
-  </si>
-  <si>
-    <t>V-shaped holder collimating lens</t>
-  </si>
-  <si>
     <t>Attachment lens to iris</t>
   </si>
   <si>
@@ -211,57 +202,24 @@
     <t>Pedestal Pillar Post BS1 (L=1'')</t>
   </si>
   <si>
-    <t>Spacer post BS1 (L=10mm)</t>
-  </si>
-  <si>
-    <t>Post BS1(L=50mm)</t>
-  </si>
-  <si>
     <t>Clamping fork for BS1 post</t>
   </si>
   <si>
     <t>SM1L03T</t>
   </si>
   <si>
-    <t>Tube Bellow BS1 to camera</t>
-  </si>
-  <si>
-    <t>Tube 1 BS1 to camera</t>
-  </si>
-  <si>
-    <t>Tube 2 BS1 to camera</t>
-  </si>
-  <si>
-    <t>Angled tube BS1 to camera</t>
-  </si>
-  <si>
     <t>SM1V10</t>
   </si>
   <si>
-    <t>Tube coupler BS1 to camera</t>
-  </si>
-  <si>
     <t>L3</t>
   </si>
   <si>
     <t>Tube with L3</t>
   </si>
   <si>
-    <t>Photodetector (Camera)</t>
-  </si>
-  <si>
-    <t>Post holder camera</t>
-  </si>
-  <si>
-    <t>Post camera</t>
-  </si>
-  <si>
     <t>Tube 1 BS1 to DCC</t>
   </si>
   <si>
-    <t>DCC</t>
-  </si>
-  <si>
     <t>SM1L20C</t>
   </si>
   <si>
@@ -298,39 +256,9 @@
     <t>DC1-DCH/M</t>
   </si>
   <si>
-    <t>Tube 1 box to DC2 with L5</t>
-  </si>
-  <si>
-    <t>Tube 2 box to DC2</t>
-  </si>
-  <si>
-    <t>Tube coupler box to DC2</t>
-  </si>
-  <si>
-    <t>Tube 3 box to DC2</t>
-  </si>
-  <si>
-    <t>Rods box to DC2 3''</t>
-  </si>
-  <si>
-    <t>2x Rod adapter box to DC2</t>
-  </si>
-  <si>
-    <t>Cage cube for DC2</t>
-  </si>
-  <si>
-    <t>Cap for spare port of DC2 cage cube</t>
-  </si>
-  <si>
     <t>UPH/30/M</t>
   </si>
   <si>
-    <t>Post Holder DC2 (L=30mm)</t>
-  </si>
-  <si>
-    <t>Post DC2 (L=30 mm)</t>
-  </si>
-  <si>
     <t>NC395323-T640lpxr</t>
   </si>
   <si>
@@ -340,24 +268,12 @@
     <t>L6</t>
   </si>
   <si>
-    <t>Tube adapter DC2 to APD0</t>
-  </si>
-  <si>
-    <t>Tube 1 DC2 to APD0</t>
-  </si>
-  <si>
     <t>AC254-75-B-ML</t>
   </si>
   <si>
     <t>SML03</t>
   </si>
   <si>
-    <t>Tube for F1 DC2 to APD0</t>
-  </si>
-  <si>
-    <t>Lens tube bellow DC1 to APD0</t>
-  </si>
-  <si>
     <t>APD0 (Excelitas)</t>
   </si>
   <si>
@@ -382,9 +298,6 @@
     <t>CM1-CC</t>
   </si>
   <si>
-    <t>Cage cube connector DC2 to filter cube</t>
-  </si>
-  <si>
     <t>Fluorescence filter cube</t>
   </si>
   <si>
@@ -430,9 +343,6 @@
     <t>Translating lens mount L7 DC2 to APD1</t>
   </si>
   <si>
-    <t>Translating lens mount L6 DC2 to APD0</t>
-  </si>
-  <si>
     <t>Parts Microscope Body</t>
   </si>
   <si>
@@ -445,27 +355,15 @@
     <t>C4W-CC</t>
   </si>
   <si>
-    <t>Cage Cube Connector M3 to DC1</t>
-  </si>
-  <si>
     <t>C4W</t>
   </si>
   <si>
-    <t>Cage Cube DC1</t>
-  </si>
-  <si>
     <t>FFM1</t>
   </si>
   <si>
-    <t>Clamp for DC1</t>
-  </si>
-  <si>
     <t>CXYZ05/M</t>
   </si>
   <si>
-    <t>Translation Mount for P1</t>
-  </si>
-  <si>
     <t>CWY1</t>
   </si>
   <si>
@@ -496,9 +394,6 @@
     <t>Adapter (Ext. SM05 Int. SM1) for P1 to Mount</t>
   </si>
   <si>
-    <t>Cap for spare DC1 cage cube ports</t>
-  </si>
-  <si>
     <t>B4CRP/M</t>
   </si>
   <si>
@@ -520,9 +415,6 @@
     <t>N1480700</t>
   </si>
   <si>
-    <t>O1 UPLSAPO60XO/1.35 WD=0.15</t>
-  </si>
-  <si>
     <t>Nanostage Z</t>
   </si>
   <si>
@@ -535,9 +427,6 @@
     <t>Laser (515nm 80 mW, 638nm 100mW)</t>
   </si>
   <si>
-    <t>Presicion mount for DC1</t>
-  </si>
-  <si>
     <t>Screws?</t>
   </si>
   <si>
@@ -619,9 +508,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Aluminium Box</t>
-  </si>
-  <si>
     <t>DM1</t>
   </si>
   <si>
@@ -631,9 +517,6 @@
     <t>P1</t>
   </si>
   <si>
-    <t>Hard Mirror between Dm1 and L4</t>
-  </si>
-  <si>
     <t>Lens before pinhole</t>
   </si>
   <si>
@@ -656,6 +539,120 @@
   </si>
   <si>
     <t>Part Nr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-shaped collimating lens holder </t>
+  </si>
+  <si>
+    <t>Collimating lens post</t>
+  </si>
+  <si>
+    <t>Post holder</t>
+  </si>
+  <si>
+    <t>Post for BS1(L=50mm)</t>
+  </si>
+  <si>
+    <t>Post spacer BS1 (L=10mm)</t>
+  </si>
+  <si>
+    <t>CCD Camera</t>
+  </si>
+  <si>
+    <t>Tube 1 BS1 to photodetector</t>
+  </si>
+  <si>
+    <t>Tube 2 BS1 to photodetector</t>
+  </si>
+  <si>
+    <t>Tube Bellow BS1 to photodector</t>
+  </si>
+  <si>
+    <t>Tube coupler BS1 to photodetector</t>
+  </si>
+  <si>
+    <t>Angled tube BS1 to photodetector</t>
+  </si>
+  <si>
+    <t>Photodetector</t>
+  </si>
+  <si>
+    <t>Post for photodetector</t>
+  </si>
+  <si>
+    <t>Machined Aluminium Box</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Cage Cube DM1</t>
+  </si>
+  <si>
+    <t>Clamp for DM1</t>
+  </si>
+  <si>
+    <t>Cap for spare DM1 cage cube ports</t>
+  </si>
+  <si>
+    <t>Cage Cube Connector M3 to DM1</t>
+  </si>
+  <si>
+    <t>Translating Mount for P1</t>
+  </si>
+  <si>
+    <t>Hard Mirror between DM1 and L4</t>
+  </si>
+  <si>
+    <t>Tube 1 box to DM2 with L5</t>
+  </si>
+  <si>
+    <t>Tube 2 box to DM2</t>
+  </si>
+  <si>
+    <t>Tube coupler box to DM2</t>
+  </si>
+  <si>
+    <t>Tube 3 box to DM2</t>
+  </si>
+  <si>
+    <t>2x Rods box to DM2 3''</t>
+  </si>
+  <si>
+    <t>2x Rod adapters box to DM2</t>
+  </si>
+  <si>
+    <t>Cage cube for DM2</t>
+  </si>
+  <si>
+    <t>Cap for spare port of DM2 cage cube</t>
+  </si>
+  <si>
+    <t>Post DM2 (L=30 mm)</t>
+  </si>
+  <si>
+    <t>Post Holder DM2 (L=30mm)</t>
+  </si>
+  <si>
+    <t>Tube 1 DM2 to APD0</t>
+  </si>
+  <si>
+    <t>Tube adapter DM2 to APD0</t>
+  </si>
+  <si>
+    <t>Translating lens mount L6 DM2 to APD0</t>
+  </si>
+  <si>
+    <t>Tube for F1 DM2 to APD0</t>
+  </si>
+  <si>
+    <t>Lens tube bellow DM1 to APD0</t>
+  </si>
+  <si>
+    <t>Cage cube connector DM2 to filter cube</t>
+  </si>
+  <si>
+    <t>Precision mount for DM1</t>
   </si>
 </sst>
 </file>
@@ -1172,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="A3:F29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,10 +1186,10 @@
   <sheetData>
     <row r="1" spans="1:11" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="2" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>0</v>
@@ -1203,24 +1200,24 @@
     </row>
     <row r="2" spans="1:11" ht="24" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="7" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>22</v>
@@ -1234,16 +1231,16 @@
         <v>21</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>34</v>
+        <v>171</v>
       </c>
       <c r="D4" s="26">
         <v>27</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>61</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1254,16 +1251,16 @@
         <v>29</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>33</v>
+        <v>172</v>
       </c>
       <c r="D5" s="26">
         <v>28</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1274,16 +1271,16 @@
         <v>23</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>32</v>
+        <v>173</v>
       </c>
       <c r="D6" s="26">
         <v>29</v>
       </c>
       <c r="E6" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="27" t="s">
         <v>57</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1294,7 +1291,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7" s="26">
         <v>30</v>
@@ -1303,7 +1300,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1323,7 +1320,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1331,19 +1328,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D9" s="26">
         <v>32</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1351,10 +1348,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10" s="26">
         <v>33</v>
@@ -1363,7 +1360,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1371,19 +1368,19 @@
         <v>8</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D11" s="26">
         <v>34</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1394,7 +1391,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D12" s="26">
         <v>35</v>
@@ -1403,7 +1400,7 @@
         <v>24</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>77</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1414,7 +1411,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D13" s="26">
         <v>36</v>
@@ -1423,7 +1420,7 @@
         <v>15</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>66</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1434,7 +1431,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14" s="26">
         <v>37</v>
@@ -1443,7 +1440,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>67</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1454,7 +1451,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D15" s="26">
         <v>38</v>
@@ -1463,7 +1460,7 @@
         <v>18</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>70</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1471,19 +1468,19 @@
         <v>13</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D16" s="26">
         <v>39</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>68</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1494,7 +1491,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D17" s="26">
         <v>40</v>
@@ -1503,7 +1500,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1514,7 +1511,7 @@
         <v>20</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D18" s="26">
         <v>41</v>
@@ -1523,7 +1520,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>65</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1531,10 +1528,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>52</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>55</v>
       </c>
       <c r="D19" s="26">
         <v>42</v>
@@ -1543,7 +1540,7 @@
         <v>25</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>73</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1551,10 +1548,10 @@
         <v>17</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D20" s="26">
         <v>43</v>
@@ -1563,7 +1560,7 @@
         <v>23</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>74</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1571,10 +1568,10 @@
         <v>18</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D21" s="26">
         <v>44</v>
@@ -1583,7 +1580,7 @@
         <v>29</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>75</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1591,19 +1588,19 @@
         <v>19</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D22" s="26">
         <v>45</v>
       </c>
       <c r="E22" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="27" t="s">
         <v>69</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1614,16 +1611,16 @@
         <v>31</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D23" s="26">
         <v>46</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1634,7 +1631,7 @@
         <v>7</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D24" s="26">
         <v>47</v>
@@ -1643,7 +1640,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1654,16 +1651,16 @@
         <v>15</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E25" s="29" t="s">
         <v>30</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1671,19 +1668,19 @@
         <v>23</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E26" s="29" t="s">
         <v>30</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1694,16 +1691,16 @@
         <v>9</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="E27" s="30">
         <v>21012</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>178</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1714,16 +1711,16 @@
         <v>3</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>179</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1731,19 +1728,19 @@
         <v>26</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>62</v>
+        <v>174</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E29" s="30">
         <v>49793</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1826,10 +1823,10 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="C59" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1849,7 +1846,7 @@
   <dimension ref="A2:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,24 +1861,24 @@
   <sheetData>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="11" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="F3" s="32" t="s">
         <v>22</v>
@@ -1892,10 +1889,10 @@
         <v>48</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="D4" s="34">
         <v>59</v>
@@ -1904,7 +1901,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1912,19 +1909,19 @@
         <v>49</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="D5" s="34">
         <v>60</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1932,19 +1929,19 @@
         <v>50</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>205</v>
+        <v>166</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="D6" s="34">
         <v>61</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1952,19 +1949,19 @@
         <v>51</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>206</v>
+        <v>167</v>
       </c>
       <c r="D7" s="34">
         <v>62</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1972,19 +1969,19 @@
         <v>52</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="D8" s="34">
         <v>63</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1992,30 +1989,30 @@
         <v>53</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>141</v>
+        <v>186</v>
       </c>
       <c r="D9" s="34">
         <v>64</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34">
         <v>54</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>157</v>
+      <c r="B10" s="24" t="s">
+        <v>8</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="D10" s="34">
         <v>65</v>
@@ -2024,27 +2021,27 @@
         <v>14</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34">
         <v>55</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>142</v>
+      <c r="B11" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>143</v>
+        <v>208</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>208</v>
+        <v>169</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>199</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2052,19 +2049,19 @@
         <v>56</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>8</v>
+        <v>110</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>156</v>
+        <v>187</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>207</v>
+        <v>168</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2072,19 +2069,19 @@
         <v>57</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>139</v>
+        <v>189</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="E13" s="39">
         <v>49792</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>202</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2092,19 +2089,19 @@
         <v>58</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>204</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2117,16 +2114,6 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-    </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="5"/>
@@ -2157,23 +2144,23 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>170</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="C29" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
       <c r="C31" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2189,8 +2176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F23"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,29 +2192,29 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="3" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>22</v>
@@ -2241,7 +2228,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>90</v>
+        <v>192</v>
       </c>
       <c r="D4" s="23">
         <v>86</v>
@@ -2250,7 +2237,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2261,7 +2248,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="D5" s="23">
         <v>87</v>
@@ -2270,7 +2257,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2281,7 +2268,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="D6" s="23">
         <v>88</v>
@@ -2290,7 +2277,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2301,16 +2288,16 @@
         <v>20</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>93</v>
+        <v>195</v>
       </c>
       <c r="D7" s="23">
         <v>89</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2321,7 +2308,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>94</v>
+        <v>196</v>
       </c>
       <c r="D8" s="23">
         <v>90</v>
@@ -2330,7 +2317,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2341,7 +2328,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>95</v>
+        <v>197</v>
       </c>
       <c r="D9" s="23">
         <v>91</v>
@@ -2350,7 +2337,7 @@
         <v>7</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2358,10 +2345,10 @@
         <v>72</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>96</v>
+        <v>198</v>
       </c>
       <c r="D10" s="23">
         <v>92</v>
@@ -2370,7 +2357,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>105</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2381,7 +2368,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>97</v>
+        <v>199</v>
       </c>
       <c r="D11" s="23">
         <v>93</v>
@@ -2390,7 +2377,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2401,7 +2388,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D12" s="23">
         <v>94</v>
@@ -2410,7 +2397,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="40" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2418,19 +2405,19 @@
         <v>75</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>99</v>
+        <v>201</v>
       </c>
       <c r="D13" s="23">
         <v>95</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2441,7 +2428,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>105</v>
+        <v>202</v>
       </c>
       <c r="D14" s="23">
         <v>96</v>
@@ -2450,7 +2437,7 @@
         <v>6</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2461,16 +2448,16 @@
         <v>18</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>104</v>
+        <v>203</v>
       </c>
       <c r="D15" s="23">
         <v>97</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2481,7 +2468,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>134</v>
+        <v>204</v>
       </c>
       <c r="D16" s="23">
         <v>98</v>
@@ -2490,7 +2477,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2498,19 +2485,19 @@
         <v>79</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>108</v>
+        <v>205</v>
       </c>
       <c r="D17" s="23">
         <v>99</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2521,16 +2508,16 @@
         <v>6</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>109</v>
+        <v>206</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="E18" s="30">
         <v>49793</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2538,19 +2525,19 @@
         <v>81</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>185</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2561,16 +2548,16 @@
         <v>1</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="E20" s="29" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="29" t="s">
-        <v>186</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2578,19 +2565,19 @@
         <v>83</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2598,19 +2585,19 @@
         <v>84</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="D22" s="42" t="s">
-        <v>182</v>
+        <v>145</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2621,16 +2608,16 @@
         <v>4</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2715,7 +2702,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>